<commit_message>
Atualizados os dados de Qualidade.docx e adicionadas as stories planejadas no documento UserStories.xlsx
</commit_message>
<xml_diff>
--- a/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
+++ b/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories Planejadas" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>Ao excluir um nó, os nós de hierarquia maior ou igual ao nó a ser excluido, também devem ser excluidos</t>
+  </si>
+  <si>
+    <t>Adicionar o módulo de EAP dentro do DotProject</t>
+  </si>
+  <si>
+    <t>Adicionar os botões relativos ao módulo EAP dentro do DotProject</t>
+  </si>
+  <si>
+    <t>Vincular a área do módulo EAP com o projeto dentro do DotProject</t>
+  </si>
+  <si>
+    <t>Definir o visual da EAP</t>
+  </si>
+  <si>
+    <t>Implementar a interface da EAP</t>
+  </si>
+  <si>
+    <t>Integrar interface com o módulo EAP</t>
+  </si>
+  <si>
+    <t>Integrar módulo EAP com o banco de dados</t>
+  </si>
+  <si>
+    <t>Gerar uma EAP</t>
+  </si>
+  <si>
+    <t>Total User Story Points</t>
   </si>
 </sst>
 </file>
@@ -111,7 +138,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -221,12 +248,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,6 +268,200 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5970394461115495E-2"/>
+          <c:y val="3.830104410968177E-2"/>
+          <c:w val="0.78826490754555667"/>
+          <c:h val="0.87527672790943911"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimadas</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Total de User Points</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'User Stories Planejadas'!$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Realizadas</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Total de User Points</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'User Stories Realizadas'!$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="40493056"/>
+        <c:axId val="88981504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="40493056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88981504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88981504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="40493056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86062245394042014"/>
+          <c:y val="0.36172351167241718"/>
+          <c:w val="0.13937754605957989"/>
+          <c:h val="0.20065822534493541"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>119060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>135923</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,23 +751,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="67.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="21.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,104 +788,116 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>21</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <f>SUM(D2:D20)</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -671,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,39 +921,45 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="92.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K1" s="11"/>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -736,7 +978,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -747,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
@@ -759,7 +1001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -770,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -782,7 +1024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -812,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -827,7 +1069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -841,8 +1083,15 @@
       <c r="E8" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D2:D20)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -857,71 +1106,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -929,10 +1132,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização do arquivo UserStories.xlsx
</commit_message>
<xml_diff>
--- a/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
+++ b/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="13395" yWindow="645" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories Planejadas" sheetId="1" r:id="rId1"/>
@@ -249,13 +249,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,7 +323,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>301</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,7 +351,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>123</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,11 +366,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="40493056"/>
-        <c:axId val="88981504"/>
+        <c:axId val="46478848"/>
+        <c:axId val="143520832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40493056"/>
+        <c:axId val="46478848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88981504"/>
+        <c:crossAx val="143520832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -387,9 +387,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88981504"/>
+        <c:axId val="143520832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -398,9 +399,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40493056"/>
+        <c:crossAx val="46478848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -434,15 +436,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
+      <xdr:colOff>171448</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>119060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66259</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>135923</xdr:rowOff>
+      <xdr:rowOff>124239</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -751,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,9 +797,6 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>13</v>
       </c>
@@ -812,9 +811,6 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
         <v>13</v>
       </c>
@@ -830,14 +826,17 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>28</v>
       </c>
       <c r="I4">
         <f>SUM(D2:D20)</f>
-        <v>301</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -848,7 +847,10 @@
         <v>23</v>
       </c>
       <c r="D5">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,7 +861,10 @@
         <v>24</v>
       </c>
       <c r="D6">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -870,7 +875,10 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -881,7 +889,10 @@
         <v>26</v>
       </c>
       <c r="D8">
-        <v>89</v>
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -892,12 +903,10 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -910,7 +919,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,10 +960,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="11"/>
+      <c r="K1" s="12"/>
       <c r="M1" t="s">
         <v>28</v>
       </c>
@@ -989,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
@@ -1012,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -1034,7 +1043,9 @@
       <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>40</v>
+      </c>
       <c r="E5" s="4">
         <v>3</v>
       </c>
@@ -1049,7 +1060,9 @@
       <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
       <c r="E6" s="4">
         <v>3</v>
       </c>
@@ -1064,7 +1077,9 @@
       <c r="C7" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>40</v>
+      </c>
       <c r="E7" s="4">
         <v>4</v>
       </c>
@@ -1079,7 +1094,9 @@
       <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
       <c r="E8" s="4">
         <v>4</v>
       </c>
@@ -1088,7 +1105,7 @@
       </c>
       <c r="I8">
         <f>SUM(D2:D20)</f>
-        <v>123</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1101,7 +1118,9 @@
       <c r="C9" s="4">
         <v>4</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
       <c r="E9" s="4">
         <v>4</v>
       </c>
@@ -1117,7 +1136,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="12"/>
+      <c r="D16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1133,7 +1152,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
atualização dos dados da tabela UserStories.xlsx
</commit_message>
<xml_diff>
--- a/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
+++ b/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13395" yWindow="645" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="13395" yWindow="645" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories Planejadas" sheetId="1" r:id="rId1"/>
@@ -366,11 +366,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="46478848"/>
-        <c:axId val="143520832"/>
+        <c:axId val="118714368"/>
+        <c:axId val="79783616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46478848"/>
+        <c:axId val="118714368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143520832"/>
+        <c:crossAx val="79783616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -387,7 +387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143520832"/>
+        <c:axId val="79783616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -399,7 +399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46478848"/>
+        <c:crossAx val="118714368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -756,7 +756,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,7 @@
         <v>40</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>40</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
         <v>20</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
         <v>100</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>40</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,16 +1125,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" s="10"/>
     </row>
@@ -1151,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizacao dos valores das user points planejadas
</commit_message>
<xml_diff>
--- a/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
+++ b/Dot Project EAP/4. System Management/Entrega Final/ze/UserStories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13395" yWindow="645" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="13395" yWindow="645" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories Planejadas" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>279</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -366,11 +366,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="70209536"/>
-        <c:axId val="42870464"/>
+        <c:axId val="74010624"/>
+        <c:axId val="43001536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70209536"/>
+        <c:axId val="74010624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42870464"/>
+        <c:crossAx val="43001536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -387,7 +387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42870464"/>
+        <c:axId val="43001536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="200"/>
@@ -399,10 +399,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70209536"/>
+        <c:crossAx val="74010624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="I4">
         <f>SUM(D2:D20)</f>
-        <v>279</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>